<commit_message>
Halved initial government reform progress for natives
</commit_message>
<xml_diff>
--- a/.archive/spreadsheets/reforms.xlsx
+++ b/.archive/spreadsheets/reforms.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Uros\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Uros\Documents\Paradox Interactive\Europa Universalis IV\mod\third_odyssey_DEV\.archive\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91CD69B2-44A8-4A83-945F-98349B3FA9FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B22946F-39D0-4F5C-95ED-56B7A421A85C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="825" yWindow="825" windowWidth="21600" windowHeight="11205" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
   <si>
     <t>Years</t>
   </si>
@@ -86,6 +86,15 @@
   </si>
   <si>
     <t>Ambition</t>
+  </si>
+  <si>
+    <t>Yearly 2</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>STD + MOD1</t>
   </si>
 </sst>
 </file>
@@ -480,10 +489,13 @@
   <dimension ref="B1:P21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="13" max="13" width="12.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="2:16" x14ac:dyDescent="0.25">
       <c r="M1" t="s">
@@ -496,7 +508,7 @@
         <v>10</v>
       </c>
       <c r="P1">
-        <v>0.25</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
@@ -504,21 +516,21 @@
         <v>8</v>
       </c>
       <c r="L2">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="M2" t="s">
         <v>8</v>
       </c>
       <c r="N2">
         <f>$L$2*N1</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="O2" t="s">
         <v>8</v>
       </c>
       <c r="P2">
         <f>$L$2*P1</f>
-        <v>3</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
@@ -541,14 +553,14 @@
       </c>
       <c r="N4">
         <f>$L$2*N3</f>
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="O4" t="s">
         <v>8</v>
       </c>
       <c r="P4">
         <f>$L$2*P3</f>
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
@@ -564,6 +576,18 @@
         <v>10</v>
       </c>
       <c r="J6" s="7"/>
+      <c r="K6" t="s">
+        <v>18</v>
+      </c>
+      <c r="L6">
+        <v>10</v>
+      </c>
+      <c r="M6" t="s">
+        <v>7</v>
+      </c>
+      <c r="N6">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="E7" s="1" t="s">
@@ -583,6 +607,13 @@
       </c>
       <c r="J7" s="2" t="s">
         <v>1</v>
+      </c>
+      <c r="M7" t="s">
+        <v>8</v>
+      </c>
+      <c r="N7">
+        <f>N6*L6</f>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.25">
@@ -651,6 +682,16 @@
         <f>SUM(I$8:I9)</f>
         <v>0</v>
       </c>
+      <c r="K9" t="s">
+        <v>19</v>
+      </c>
+      <c r="M9" t="s">
+        <v>20</v>
+      </c>
+      <c r="N9">
+        <f>N7+L2</f>
+        <v>11</v>
+      </c>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
@@ -664,27 +705,27 @@
       </c>
       <c r="E10" s="1">
         <f t="shared" si="0"/>
-        <v>12.5</v>
+        <v>25</v>
       </c>
       <c r="F10" s="2">
         <f>SUM(E$8:$E10)</f>
-        <v>12.5</v>
+        <v>25</v>
       </c>
       <c r="G10" s="1">
         <f t="shared" ref="G10:G12" si="2">D10/$N$2</f>
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="H10" s="2">
         <f>SUM(G$8:G10)</f>
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="I10" s="1">
         <f t="shared" ref="I10:I11" si="3">$D10/$P$2</f>
-        <v>50</v>
+        <v>33.333333333333336</v>
       </c>
       <c r="J10" s="2">
         <f>SUM(I$8:I10)</f>
-        <v>50</v>
+        <v>33.333333333333336</v>
       </c>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
@@ -699,27 +740,27 @@
       </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>16.666666666666668</v>
+        <v>33.333333333333336</v>
       </c>
       <c r="F11" s="2">
         <f>SUM(E$8:$E11)</f>
-        <v>29.166666666666668</v>
+        <v>58.333333333333336</v>
       </c>
       <c r="G11" s="1">
         <f t="shared" si="2"/>
-        <v>33.333333333333336</v>
+        <v>66.666666666666671</v>
       </c>
       <c r="H11" s="2">
         <f>SUM(G$8:G11)</f>
-        <v>58.333333333333336</v>
+        <v>116.66666666666667</v>
       </c>
       <c r="I11" s="1">
         <f t="shared" si="3"/>
-        <v>66.666666666666671</v>
+        <v>44.444444444444443</v>
       </c>
       <c r="J11" s="2">
         <f>SUM(I$8:I11)</f>
-        <v>116.66666666666667</v>
+        <v>77.777777777777771</v>
       </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
@@ -733,28 +774,28 @@
         <v>250</v>
       </c>
       <c r="E12" s="1">
-        <f t="shared" si="0"/>
-        <v>20.833333333333332</v>
+        <f>D12/$N$9</f>
+        <v>22.727272727272727</v>
       </c>
       <c r="F12" s="2">
         <f>SUM(E$8:$E12)</f>
-        <v>50</v>
+        <v>81.060606060606062</v>
       </c>
       <c r="G12" s="1">
         <f t="shared" si="2"/>
-        <v>41.666666666666664</v>
+        <v>83.333333333333329</v>
       </c>
       <c r="H12" s="2">
         <f>SUM(G$8:G12)</f>
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="I12" s="1">
         <f>$D12/$P$2</f>
-        <v>83.333333333333329</v>
+        <v>55.555555555555557</v>
       </c>
       <c r="J12" s="2">
         <f>SUM(I$8:I12)</f>
-        <v>200</v>
+        <v>133.33333333333331</v>
       </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
@@ -768,25 +809,25 @@
         <v>300</v>
       </c>
       <c r="E13" s="1">
-        <f t="shared" si="0"/>
-        <v>25</v>
+        <f>D13/$N$9</f>
+        <v>27.272727272727273</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="1">
-        <f>$D13/$N$4</f>
-        <v>25</v>
+        <f>$D13/$N$9</f>
+        <v>27.272727272727273</v>
       </c>
       <c r="H13" s="2">
         <f>SUM(G$13:G13)</f>
-        <v>25</v>
+        <v>27.272727272727273</v>
       </c>
       <c r="I13" s="1">
         <f>$D13/$P$4</f>
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="J13" s="2">
         <f>SUM(I$13:I13)</f>
-        <v>25</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
@@ -800,25 +841,25 @@
         <v>350</v>
       </c>
       <c r="E14" s="1">
-        <f t="shared" si="0"/>
-        <v>29.166666666666668</v>
+        <f t="shared" ref="E14:E17" si="4">D14/$N$9</f>
+        <v>31.818181818181817</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="1">
-        <f t="shared" ref="G14:G17" si="4">$D14/$N$4</f>
-        <v>29.166666666666668</v>
+        <f t="shared" ref="G14:G17" si="5">$D14/$N$9</f>
+        <v>31.818181818181817</v>
       </c>
       <c r="H14" s="2">
         <f>SUM(G$13:G14)</f>
-        <v>54.166666666666671</v>
+        <v>59.090909090909093</v>
       </c>
       <c r="I14" s="1">
-        <f t="shared" ref="I14:I17" si="5">$D14/$P$4</f>
-        <v>29.166666666666668</v>
+        <f t="shared" ref="I14:I17" si="6">$D14/$P$4</f>
+        <v>58.333333333333336</v>
       </c>
       <c r="J14" s="2">
         <f>SUM(I$13:I14)</f>
-        <v>54.166666666666671</v>
+        <v>108.33333333333334</v>
       </c>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
@@ -832,25 +873,25 @@
         <v>400</v>
       </c>
       <c r="E15" s="1">
-        <f t="shared" si="0"/>
-        <v>33.333333333333336</v>
+        <f t="shared" si="4"/>
+        <v>36.363636363636367</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="1">
-        <f t="shared" si="4"/>
-        <v>33.333333333333336</v>
+        <f t="shared" si="5"/>
+        <v>36.363636363636367</v>
       </c>
       <c r="H15" s="2">
         <f>SUM(G$13:G15)</f>
-        <v>87.5</v>
+        <v>95.454545454545467</v>
       </c>
       <c r="I15" s="1">
-        <f t="shared" si="5"/>
-        <v>33.333333333333336</v>
+        <f t="shared" si="6"/>
+        <v>66.666666666666671</v>
       </c>
       <c r="J15" s="2">
         <f>SUM(I$13:I15)</f>
-        <v>87.5</v>
+        <v>175</v>
       </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
@@ -864,25 +905,25 @@
         <v>450</v>
       </c>
       <c r="E16" s="1">
-        <f t="shared" si="0"/>
-        <v>37.5</v>
+        <f t="shared" si="4"/>
+        <v>40.909090909090907</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="1">
-        <f t="shared" si="4"/>
-        <v>37.5</v>
+        <f t="shared" si="5"/>
+        <v>40.909090909090907</v>
       </c>
       <c r="H16" s="2">
         <f>SUM(G$13:G16)</f>
-        <v>125</v>
+        <v>136.36363636363637</v>
       </c>
       <c r="I16" s="1">
-        <f t="shared" si="5"/>
-        <v>37.5</v>
+        <f t="shared" si="6"/>
+        <v>75</v>
       </c>
       <c r="J16" s="2">
         <f>SUM(I$13:I16)</f>
-        <v>125</v>
+        <v>250</v>
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
@@ -895,26 +936,26 @@
       <c r="D17">
         <v>500</v>
       </c>
-      <c r="E17" s="3">
-        <f t="shared" si="0"/>
-        <v>41.666666666666664</v>
+      <c r="E17" s="1">
+        <f t="shared" si="4"/>
+        <v>45.454545454545453</v>
       </c>
       <c r="F17" s="4"/>
-      <c r="G17" s="3">
-        <f t="shared" si="4"/>
-        <v>41.666666666666664</v>
+      <c r="G17" s="1">
+        <f t="shared" si="5"/>
+        <v>45.454545454545453</v>
       </c>
       <c r="H17" s="4">
         <f>SUM(G$13:G17)</f>
-        <v>166.66666666666666</v>
+        <v>181.81818181818181</v>
       </c>
       <c r="I17" s="3">
-        <f t="shared" si="5"/>
-        <v>41.666666666666664</v>
+        <f t="shared" si="6"/>
+        <v>83.333333333333329</v>
       </c>
       <c r="J17" s="2">
         <f>SUM(I$13:I17)</f>
-        <v>166.66666666666666</v>
+        <v>333.33333333333331</v>
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">

</xml_diff>